<commit_message>
📊 Arribos 141 actualizados - 5
</commit_message>
<xml_diff>
--- a/data/arribos-141.xlsx
+++ b/data/arribos-141.xlsx
@@ -473,17 +473,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>09/01/2026 14:44:22</t>
+          <t>09/01/2026 14:50:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>14:44</t>
+          <t>14:50</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>14:49</t>
+          <t>14:55</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -500,17 +500,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>09/01/2026 14:44:22</t>
+          <t>09/01/2026 14:50:00</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>14:44</t>
+          <t>14:50</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>14:59</t>
+          <t>15:05</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -535,17 +535,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>09/01/2026 14:44:22</t>
+          <t>09/01/2026 14:50:00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>14:44</t>
+          <t>14:50</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>15:10</t>
+          <t>15:16</t>
         </is>
       </c>
       <c r="D4" t="n">

</xml_diff>

<commit_message>
📊 Arribos 141 actualizados - 6
</commit_message>
<xml_diff>
--- a/data/arribos-141.xlsx
+++ b/data/arribos-141.xlsx
@@ -473,17 +473,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>09/01/2026 14:50:00</t>
+          <t>09/01/2026 14:53:13</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>14:50</t>
+          <t>14:53</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>14:55</t>
+          <t>14:58</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -500,17 +500,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>09/01/2026 14:50:00</t>
+          <t>09/01/2026 14:53:13</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>14:50</t>
+          <t>14:53</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>15:05</t>
+          <t>15:08</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -535,17 +535,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>09/01/2026 14:50:00</t>
+          <t>09/01/2026 14:53:13</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>14:50</t>
+          <t>14:53</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>15:16</t>
+          <t>15:19</t>
         </is>
       </c>
       <c r="D4" t="n">

</xml_diff>

<commit_message>
📊 Arribos 141 actualizados - 7
</commit_message>
<xml_diff>
--- a/data/arribos-141.xlsx
+++ b/data/arribos-141.xlsx
@@ -473,17 +473,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>09/01/2026 14:53:13</t>
+          <t>09/01/2026 14:55:29</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>14:55</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>14:58</t>
+          <t>15:00</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -500,17 +500,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>09/01/2026 14:53:13</t>
+          <t>09/01/2026 14:55:29</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>14:55</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>15:08</t>
+          <t>15:10</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -535,17 +535,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>09/01/2026 14:53:13</t>
+          <t>09/01/2026 14:55:29</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>14:53</t>
+          <t>14:55</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>15:19</t>
+          <t>15:21</t>
         </is>
       </c>
       <c r="D4" t="n">

</xml_diff>